<commit_message>
Correct english translations for spanish and greek translated content Update tutorial positioning and some text to be easier to understand Localize text in the tutorial
</commit_message>
<xml_diff>
--- a/Assets/Editor/Strings/StringFile.xlsx
+++ b/Assets/Editor/Strings/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="534">
   <si>
     <t>XXXX</t>
   </si>
@@ -1482,13 +1482,157 @@
   </si>
   <si>
     <t>Ζητήστε πληροφορίες από τους πολίτες!</t>
+  </si>
+  <si>
+    <t>TUTORIAL_TEXT_1</t>
+  </si>
+  <si>
+    <t>TUTORIAL_TEXT_2</t>
+  </si>
+  <si>
+    <t>TUTORIAL_TEXT_3</t>
+  </si>
+  <si>
+    <t>TUTORIAL_TEXT_4</t>
+  </si>
+  <si>
+    <t>TUTORIAL_TEXT_5</t>
+  </si>
+  <si>
+    <t>TUTORIAL_TEXT_6</t>
+  </si>
+  <si>
+    <t>TUTORIAL_TEXT_7</t>
+  </si>
+  <si>
+    <t>TUTORIAL_TEXT_8</t>
+  </si>
+  <si>
+    <t>In some cases, you might not have enough information to act upon.\n\nTry asking citizens for some more information.</t>
+  </si>
+  <si>
+    <t>In Resource Force, It is your job to decide how to handle incoming reports.\n\nMake sure to read each report carefully, they may be best ignored.</t>
+  </si>
+  <si>
+    <t>When an incident has been handled, you will be given an update of what happened and how it effects public satisfcation.</t>
+  </si>
+  <si>
+    <t>The severity of this incident has increased.\n\nNow it's your turn. Read the description above and try to make the best choice.</t>
+  </si>
+  <si>
+    <t>For every choice you make, public satisfaction will be affected.\n\nThis is indicated at the top of the screen.</t>
+  </si>
+  <si>
+    <t>The game is lost when satisfaction is below 10% at the end of the turn.\n\nNow that the basics have been covered you should be ready to take on the task of running the police force.\n\nHow many turns can you survive?</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_1_TITLE</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_1_REPORT</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_1_FEEDBACK</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>A man has been seen dropping litter</t>
+  </si>
+  <si>
+    <t>Good job! Police should not deal with this type of incident</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_2_TITLE</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_2_REPORT</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_2_FEEDBACK</t>
+  </si>
+  <si>
+    <t>Harassment Report</t>
+  </si>
+  <si>
+    <t>Reports of an unidentified person harassing neighbours</t>
+  </si>
+  <si>
+    <t>Great! You should try to get more information before deploying officers</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_3_TITLE</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_3_REPORT</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_3_FEEDBACK</t>
+  </si>
+  <si>
+    <t>Man with knife</t>
+  </si>
+  <si>
+    <t>A man has been seen in the city centre threatening people with a knife</t>
+  </si>
+  <si>
+    <t>Officers required to make sure nobody gets hurt</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_4_TITLE</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_4_REPORT</t>
+  </si>
+  <si>
+    <t>Information Forwarded</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_5_TITLE</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_5_REPORT</t>
+  </si>
+  <si>
+    <t>Information Received</t>
+  </si>
+  <si>
+    <t>Citizens provided a full descruption along with reports of assault, the exact location is unknown</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_5_FEEDBACK_WAIT</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_5_FEEDBACK_CITIZEN</t>
+  </si>
+  <si>
+    <t>TUTORIAL_INCIDENT_5_FEEDBACK_OFFICER</t>
+  </si>
+  <si>
+    <t>Bad Idea, you should have sent officers to prevent further altercation</t>
+  </si>
+  <si>
+    <t>Ok, you might be able to get a location, but you may be putting citizens at risk</t>
+  </si>
+  <si>
+    <t>Well Done! Officers need to be sent to make sure that nobody gets hurt</t>
+  </si>
+  <si>
+    <t>Information of man seen dropping litter has been passed onto the local council</t>
+  </si>
+  <si>
+    <t>In reports where people may be in danger, it is important to send officers.\n\nThis incident requires 2 officers for 2 turns, as indicated on the button below</t>
+  </si>
+  <si>
+    <t>At the end of each turn, you are shown a summary of how well you have done.\n\nEvery turn has a number of incidents that you must review. Your 2 officers are still dispatched and won't return until another turn has been completed, as shown by the number on each officer icon.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1516,8 +1660,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1538,6 +1689,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1565,12 +1721,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1606,10 +1763,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1889,10 +2050,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3707,6 +3868,414 @@
         <v>0</v>
       </c>
     </row>
+    <row r="107" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A107" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>495</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A108" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="B108" s="13" t="s">
+        <v>494</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A109" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="B109" s="13" t="s">
+        <v>532</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A110" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="B110" s="13" t="s">
+        <v>533</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A111" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="B111" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A112" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="B112" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A113" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="B113" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A114" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="B114" s="13" t="s">
+        <v>499</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="B115" s="13" t="s">
+        <v>503</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="B116" s="13" t="s">
+        <v>504</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="B117" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="B118" s="13" t="s">
+        <v>509</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="B119" s="13" t="s">
+        <v>510</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A120" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="B120" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A121" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="B121" s="13" t="s">
+        <v>515</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="B122" s="13" t="s">
+        <v>516</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="B123" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="B124" s="13" t="s">
+        <v>520</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A125" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="B125" s="13" t="s">
+        <v>531</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="B126" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A127" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="B127" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A128" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="B128" s="13" t="s">
+        <v>528</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A129" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="B129" s="13" t="s">
+        <v>529</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A130" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="B130" s="13" t="s">
+        <v>530</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Change "select" to "select location" remove "no new content found" and just go straight to game "Tap to start" moved to be located on a button, to stop players starting the game again after going to the menu Increased fade on buttons during feedback so they dont look interactable Made citizen animation green to match button
</commit_message>
<xml_diff>
--- a/Assets/Editor/Strings/StringFile.xlsx
+++ b/Assets/Editor/Strings/StringFile.xlsx
@@ -53,9 +53,6 @@
     <t>START_SCREEN_TAP</t>
   </si>
   <si>
-    <t>Tap to start!</t>
-  </si>
-  <si>
     <t>BASIC_TEXT_OK</t>
   </si>
   <si>
@@ -1626,13 +1623,16 @@
   </si>
   <si>
     <t>At the end of each turn, you are shown a summary of how well you have done.\n\nEvery turn has a number of incidents that you must review. Your 2 officers are still dispatched and won't return until another turn has been completed, as shown by the number on each officer icon.</t>
+  </si>
+  <si>
+    <t>Tap here to start!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1660,15 +1660,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1689,11 +1682,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1721,13 +1709,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1745,9 +1732,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -1763,14 +1747,19 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2052,8 +2041,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G110" sqref="G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2088,16 +2077,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>287</v>
+        <v>471</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2105,16 +2094,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2122,1608 +2111,1608 @@
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>122</v>
+        <v>533</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>11</v>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>288</v>
+        <v>10</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>338</v>
+      <c r="C6" s="7" t="s">
+        <v>337</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>289</v>
+        <v>213</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>339</v>
+      <c r="C7" s="7" t="s">
+        <v>338</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>290</v>
+        <v>214</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>340</v>
+      <c r="C8" s="7" t="s">
+        <v>339</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>123</v>
+        <v>215</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>341</v>
+        <v>50</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>340</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>291</v>
+        <v>216</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>342</v>
+        <v>49</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>341</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>292</v>
+        <v>217</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>482</v>
+      <c r="E11" s="7" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>343</v>
+      <c r="C12" s="7" t="s">
+        <v>342</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>124</v>
+        <v>218</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>344</v>
+      <c r="C13" s="7" t="s">
+        <v>343</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>293</v>
+        <v>219</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>345</v>
+      <c r="C14" s="7" t="s">
+        <v>344</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>294</v>
+        <v>220</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>346</v>
+        <v>19</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>345</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>125</v>
+        <v>221</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>347</v>
+        <v>20</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>346</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>295</v>
+        <v>222</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>348</v>
+        <v>21</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>347</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>126</v>
+        <v>223</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>349</v>
+        <v>22</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>348</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>127</v>
+        <v>224</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>350</v>
+      <c r="C19" s="7" t="s">
+        <v>349</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>128</v>
+        <v>225</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>351</v>
+      <c r="C20" s="7" t="s">
+        <v>350</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>296</v>
+        <v>226</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>352</v>
+      <c r="C21" s="7" t="s">
+        <v>351</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>297</v>
+        <v>227</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>353</v>
+      <c r="C22" s="7" t="s">
+        <v>352</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>129</v>
+        <v>228</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>354</v>
+      <c r="C23" s="7" t="s">
+        <v>353</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>298</v>
+        <v>229</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>299</v>
+        <v>230</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="8" t="s">
         <v>454</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>355</v>
+        <v>36</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>354</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>130</v>
+        <v>231</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>356</v>
+        <v>130</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>355</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>300</v>
+        <v>232</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>357</v>
+      <c r="C28" s="7" t="s">
+        <v>356</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>301</v>
+        <v>233</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>358</v>
+      <c r="C29" s="7" t="s">
+        <v>357</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>302</v>
+        <v>234</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>359</v>
+        <v>59</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>358</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>132</v>
+        <v>235</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>153</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>165</v>
+        <v>236</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>360</v>
+        <v>84</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>359</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>133</v>
+        <v>237</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>204</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>362</v>
+      <c r="C34" s="7" t="s">
+        <v>361</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>303</v>
+        <v>239</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>363</v>
+      <c r="C35" s="7" t="s">
+        <v>362</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>304</v>
+        <v>240</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>364</v>
+        <v>83</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>363</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>305</v>
+        <v>241</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>57</v>
+      <c r="C37" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>134</v>
+        <v>242</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>59</v>
+      <c r="C38" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>135</v>
+        <v>243</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>365</v>
+      <c r="C39" s="7" t="s">
+        <v>364</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>136</v>
+        <v>244</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>366</v>
+      <c r="C40" s="7" t="s">
+        <v>365</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>306</v>
+        <v>245</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>367</v>
+        <v>53</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>366</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>137</v>
+        <v>246</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>368</v>
+        <v>148</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>367</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>307</v>
+        <v>247</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>369</v>
+        <v>90</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>368</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>308</v>
+        <v>248</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>370</v>
+        <v>91</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>369</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>309</v>
+        <v>249</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>371</v>
+      <c r="C45" s="7" t="s">
+        <v>370</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>310</v>
+        <v>250</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>372</v>
+      <c r="C46" s="7" t="s">
+        <v>371</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>138</v>
+        <v>251</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>100</v>
+      <c r="C47" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>139</v>
+        <v>252</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>373</v>
+      <c r="C48" s="7" t="s">
+        <v>372</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>311</v>
+        <v>253</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>374</v>
+      <c r="C49" s="7" t="s">
+        <v>373</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>164</v>
+        <v>254</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E50" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>376</v>
+        <v>175</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>375</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>312</v>
+        <v>256</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>377</v>
+        <v>178</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>376</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>313</v>
+        <v>257</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>378</v>
+        <v>176</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>377</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>314</v>
+        <v>258</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>379</v>
+        <v>179</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>378</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>315</v>
+        <v>259</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>380</v>
+        <v>177</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>379</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>316</v>
+        <v>260</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="C56" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E56" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>382</v>
+        <v>202</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>381</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>317</v>
+        <v>262</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>383</v>
+      <c r="C58" s="7" t="s">
+        <v>382</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>318</v>
+        <v>263</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>384</v>
+      <c r="C59" s="7" t="s">
+        <v>383</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>319</v>
+        <v>264</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>385</v>
+      <c r="C60" s="7" t="s">
+        <v>384</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>320</v>
+        <v>265</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>386</v>
+      <c r="C61" s="7" t="s">
+        <v>385</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>321</v>
+        <v>266</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>387</v>
+      <c r="C62" s="7" t="s">
+        <v>386</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>322</v>
+        <v>267</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>388</v>
+      <c r="C63" s="7" t="s">
+        <v>387</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>323</v>
+        <v>268</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>389</v>
+      <c r="C64" s="7" t="s">
+        <v>388</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>324</v>
+        <v>269</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>390</v>
+        <v>76</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>389</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>325</v>
+        <v>270</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>391</v>
+      <c r="C66" s="7" t="s">
+        <v>390</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="E66" s="8" t="s">
-        <v>326</v>
+        <v>271</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>392</v>
+      <c r="C67" s="7" t="s">
+        <v>391</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>327</v>
+        <v>272</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>393</v>
+        <v>200</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>392</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>328</v>
+        <v>273</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="C69" s="8" t="s">
         <v>450</v>
       </c>
+      <c r="C69" s="7" t="s">
+        <v>449</v>
+      </c>
       <c r="D69" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="E69" s="9" t="s">
         <v>448</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="C70" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="D70" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="E70" s="8" t="s">
         <v>446</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="C71" s="8" t="s">
         <v>442</v>
       </c>
+      <c r="C71" s="7" t="s">
+        <v>441</v>
+      </c>
       <c r="D71" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="E71" s="8" t="s">
         <v>440</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>394</v>
+      <c r="C72" s="7" t="s">
+        <v>393</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="E72" s="7" t="s">
-        <v>329</v>
+        <v>274</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>395</v>
+        <v>107</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>394</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="E73" s="8" t="s">
-        <v>330</v>
+        <v>275</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>396</v>
+      <c r="C74" s="7" t="s">
+        <v>395</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>331</v>
+        <v>276</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>355</v>
+        <v>36</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>354</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>130</v>
+        <v>231</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>397</v>
+      <c r="C76" s="7" t="s">
+        <v>396</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>163</v>
+        <v>277</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="C77" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="E77" s="6" t="s">
         <v>437</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B78" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="D78" s="5" t="s">
         <v>433</v>
       </c>
-      <c r="C78" s="8" t="s">
-        <v>432</v>
-      </c>
-      <c r="D78" s="5" t="s">
+      <c r="E78" s="6" t="s">
         <v>434</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B79" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>399</v>
+      <c r="C80" s="7" t="s">
+        <v>398</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>332</v>
+        <v>279</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B81" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>118</v>
+      <c r="C81" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E81" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>120</v>
+      <c r="C82" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E82" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>400</v>
+        <v>141</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>399</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>162</v>
+        <v>280</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>401</v>
+        <v>142</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>400</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>333</v>
+        <v>278</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>431</v>
+        <v>411</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>430</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="E85" s="9" t="s">
         <v>429</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="C86" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="E86" s="7" t="s">
         <v>427</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="E86" s="8" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>426</v>
+        <v>408</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>425</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="E87" s="8" t="s">
         <v>424</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="C88" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="D88" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="E88" s="7" t="s">
         <v>422</v>
-      </c>
-      <c r="E88" s="8" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>420</v>
+        <v>407</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>419</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="E89" s="8" t="s">
         <v>417</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>419</v>
+        <v>405</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>418</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="E90" s="8" t="s">
-        <v>416</v>
+        <v>413</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="C91" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="E91" s="7" t="s">
         <v>414</v>
-      </c>
-      <c r="E91" s="8" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>202</v>
+        <v>167</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="E92" s="10" t="s">
-        <v>334</v>
+        <v>281</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>402</v>
+        <v>192</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>401</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="E93" s="10" t="s">
-        <v>196</v>
+        <v>282</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>350</v>
+        <v>24</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>349</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="E94" s="10" t="s">
-        <v>128</v>
+        <v>225</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>403</v>
+        <v>193</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>402</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>197</v>
+        <v>283</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>404</v>
+        <v>194</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>403</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="E96" s="10" t="s">
-        <v>198</v>
+        <v>284</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B97" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B97" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>405</v>
+      <c r="C97" s="7" t="s">
+        <v>404</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="E97" s="10" t="s">
-        <v>335</v>
+        <v>285</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="B98" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="B98" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="C98" s="12" t="s">
-        <v>473</v>
+      <c r="C98" s="11" t="s">
+        <v>472</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>0</v>
@@ -3734,13 +3723,13 @@
     </row>
     <row r="99" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="C99" s="12" t="s">
-        <v>474</v>
+        <v>469</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>473</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>0</v>
@@ -3751,13 +3740,13 @@
     </row>
     <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B100" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B100" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C100" s="12" t="s">
-        <v>475</v>
+      <c r="C100" s="11" t="s">
+        <v>474</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>0</v>
@@ -3768,13 +3757,13 @@
     </row>
     <row r="101" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="B101" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="B101" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="C101" s="12" t="s">
-        <v>476</v>
+      <c r="C101" s="11" t="s">
+        <v>475</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>0</v>
@@ -3785,13 +3774,13 @@
     </row>
     <row r="102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="C102" s="12" t="s">
-        <v>477</v>
+        <v>457</v>
+      </c>
+      <c r="C102" s="11" t="s">
+        <v>476</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>0</v>
@@ -3802,13 +3791,13 @@
     </row>
     <row r="103" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="B103" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="B103" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="C103" s="12" t="s">
-        <v>478</v>
+      <c r="C103" s="11" t="s">
+        <v>477</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>0</v>
@@ -3819,13 +3808,13 @@
     </row>
     <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B104" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="B104" s="5" t="s">
-        <v>463</v>
-      </c>
-      <c r="C104" s="12" t="s">
-        <v>479</v>
+      <c r="C104" s="11" t="s">
+        <v>478</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>0</v>
@@ -3836,13 +3825,13 @@
     </row>
     <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="C105" s="12" t="s">
-        <v>480</v>
+      <c r="C105" s="11" t="s">
+        <v>479</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>0</v>
@@ -3853,13 +3842,13 @@
     </row>
     <row r="106" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="B106" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="B106" s="5" t="s">
-        <v>467</v>
-      </c>
-      <c r="C106" s="12" t="s">
-        <v>481</v>
+      <c r="C106" s="11" t="s">
+        <v>480</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>0</v>
@@ -3870,10 +3859,10 @@
     </row>
     <row r="107" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A107" s="4" t="s">
-        <v>486</v>
-      </c>
-      <c r="B107" s="13" t="s">
-        <v>495</v>
+        <v>485</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>494</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>0</v>
@@ -3887,10 +3876,10 @@
     </row>
     <row r="108" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A108" s="4" t="s">
-        <v>487</v>
-      </c>
-      <c r="B108" s="13" t="s">
-        <v>494</v>
+        <v>486</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>493</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>0</v>
@@ -3904,10 +3893,10 @@
     </row>
     <row r="109" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="B109" s="13" t="s">
-        <v>532</v>
+        <v>487</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>531</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>0</v>
@@ -3921,10 +3910,10 @@
     </row>
     <row r="110" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="B110" s="13" t="s">
-        <v>533</v>
+        <v>488</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>532</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>0</v>
@@ -3938,10 +3927,10 @@
     </row>
     <row r="111" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="B111" s="13" t="s">
-        <v>496</v>
+        <v>489</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>495</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>0</v>
@@ -3955,10 +3944,10 @@
     </row>
     <row r="112" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="B112" s="13" t="s">
-        <v>497</v>
+        <v>490</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>496</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>0</v>
@@ -3972,10 +3961,10 @@
     </row>
     <row r="113" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A113" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="B113" s="13" t="s">
-        <v>498</v>
+        <v>491</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>0</v>
@@ -3989,10 +3978,10 @@
     </row>
     <row r="114" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="B114" s="13" t="s">
-        <v>499</v>
+        <v>492</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>498</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>0</v>
@@ -4006,10 +3995,10 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
-        <v>500</v>
-      </c>
-      <c r="B115" s="13" t="s">
-        <v>503</v>
+        <v>499</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>502</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>0</v>
@@ -4023,10 +4012,10 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="B116" s="13" t="s">
-        <v>504</v>
+        <v>500</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>503</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>0</v>
@@ -4040,10 +4029,10 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
-        <v>502</v>
-      </c>
-      <c r="B117" s="13" t="s">
-        <v>505</v>
+        <v>501</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>504</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>0</v>
@@ -4057,10 +4046,10 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="B118" s="13" t="s">
-        <v>509</v>
+        <v>505</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>508</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>0</v>
@@ -4074,10 +4063,10 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="B119" s="13" t="s">
-        <v>510</v>
+        <v>506</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>509</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>0</v>
@@ -4091,10 +4080,10 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
-        <v>508</v>
-      </c>
-      <c r="B120" s="13" t="s">
-        <v>511</v>
+        <v>507</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>510</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>0</v>
@@ -4108,10 +4097,10 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="B121" s="13" t="s">
-        <v>515</v>
+        <v>511</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>514</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>0</v>
@@ -4125,10 +4114,10 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
-        <v>513</v>
-      </c>
-      <c r="B122" s="13" t="s">
-        <v>516</v>
+        <v>512</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>515</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>0</v>
@@ -4142,10 +4131,10 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="B123" s="13" t="s">
-        <v>517</v>
+        <v>513</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>516</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>0</v>
@@ -4159,10 +4148,10 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="B124" s="13" t="s">
-        <v>520</v>
+        <v>517</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>519</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>0</v>
@@ -4176,10 +4165,10 @@
     </row>
     <row r="125" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
-        <v>519</v>
-      </c>
-      <c r="B125" s="13" t="s">
-        <v>531</v>
+        <v>518</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>530</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>0</v>
@@ -4193,10 +4182,10 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="B126" s="13" t="s">
-        <v>523</v>
+        <v>520</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>522</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>0</v>
@@ -4210,10 +4199,10 @@
     </row>
     <row r="127" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
-        <v>522</v>
-      </c>
-      <c r="B127" s="13" t="s">
-        <v>524</v>
+        <v>521</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>523</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>0</v>
@@ -4227,10 +4216,10 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
-        <v>525</v>
-      </c>
-      <c r="B128" s="13" t="s">
-        <v>528</v>
+        <v>524</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>527</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>0</v>
@@ -4244,10 +4233,10 @@
     </row>
     <row r="129" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
-        <v>526</v>
-      </c>
-      <c r="B129" s="13" t="s">
-        <v>529</v>
+        <v>525</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>528</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>0</v>
@@ -4261,10 +4250,10 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="B130" s="13" t="s">
-        <v>530</v>
+        <v>526</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>529</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
default text to english, change citizen icon in tutorial to also be green update typos in spreadsheet
</commit_message>
<xml_diff>
--- a/Assets/Editor/Strings/StringFile.xlsx
+++ b/Assets/Editor/Strings/StringFile.xlsx
@@ -221,9 +221,6 @@
     <t>TUTORIAL_TEXT_TOP_BAR</t>
   </si>
   <si>
-    <t>The top of the screen shows the current satisfaction status, the further into red you go, the closer you are to losing. Solve cases to stay out of the red</t>
-  </si>
-  <si>
     <t>TUTORIAL_TEXT_STATUS_BAR</t>
   </si>
   <si>
@@ -236,24 +233,15 @@
     <t>TUTORIAL_TEXT_INFORMATION</t>
   </si>
   <si>
-    <t>This box will give you information on the current case and keep you updated on its status</t>
-  </si>
-  <si>
     <t>TUTORIAL_TEXT_INCIDENTS</t>
   </si>
   <si>
     <t>TUTORIAL_TEXT_BUTTONS</t>
   </si>
   <si>
-    <t>Each case can have up to 3 options, wait for more officers, send the required officers or ask citizens for help when available</t>
-  </si>
-  <si>
     <t>TUTORIAL_TEXT_OFFICER_REQ</t>
   </si>
   <si>
-    <t>Each case will need a number of officers to attend  for a set number of turns</t>
-  </si>
-  <si>
     <t>The officer indicator informs you how many officers are available and how many turns until officers in the field return and become available again</t>
   </si>
   <si>
@@ -1241,12 +1229,6 @@
     <t>Meldt een scenario probleem</t>
   </si>
   <si>
-    <t>{0} Turn Survived\nEach turn will consist of a number of cases with choices to make</t>
-  </si>
-  <si>
-    <t>{0} Turns Survived\nEach turn will consist of a number of cases with choices to make</t>
-  </si>
-  <si>
     <t>{0} Officers Available\nA limited number available so be careful, you never know when a severe incident may occur</t>
   </si>
   <si>
@@ -1397,9 +1379,6 @@
     <t>Retrieving Content…</t>
   </si>
   <si>
-    <t xml:space="preserve">Checking For New Content… </t>
-  </si>
-  <si>
     <t>BASIC_TEXT_CHECKING_NEW_CONTENT</t>
   </si>
   <si>
@@ -1472,9 +1451,6 @@
     <t>¡Pide información a los ciudadanos!</t>
   </si>
   <si>
-    <t>Ask citizens for information!</t>
-  </si>
-  <si>
     <t>Vraag burgers om informatie!</t>
   </si>
   <si>
@@ -1505,12 +1481,6 @@
     <t>TUTORIAL_TEXT_8</t>
   </si>
   <si>
-    <t>In some cases, you might not have enough information to act upon.\n\nTry asking citizens for some more information.</t>
-  </si>
-  <si>
-    <t>In Resource Force, It is your job to decide how to handle incoming reports.\n\nMake sure to read each report carefully, they may be best ignored.</t>
-  </si>
-  <si>
     <t>When an incident has been handled, you will be given an update of what happened and how it effects public satisfcation.</t>
   </si>
   <si>
@@ -1532,9 +1502,6 @@
     <t>TUTORIAL_INCIDENT_1_FEEDBACK</t>
   </si>
   <si>
-    <t>Report</t>
-  </si>
-  <si>
     <t>A man has been seen dropping litter</t>
   </si>
   <si>
@@ -1550,12 +1517,6 @@
     <t>TUTORIAL_INCIDENT_2_FEEDBACK</t>
   </si>
   <si>
-    <t>Harassment Report</t>
-  </si>
-  <si>
-    <t>Reports of an unidentified person harassing neighbours</t>
-  </si>
-  <si>
     <t>Great! You should try to get more information before deploying officers</t>
   </si>
   <si>
@@ -1595,9 +1556,6 @@
     <t>Information Received</t>
   </si>
   <si>
-    <t>Citizens provided a full descruption along with reports of assault, the exact location is unknown</t>
-  </si>
-  <si>
     <t>TUTORIAL_INCIDENT_5_FEEDBACK_WAIT</t>
   </si>
   <si>
@@ -1619,13 +1577,55 @@
     <t>Information of man seen dropping litter has been passed onto the local council</t>
   </si>
   <si>
-    <t>In reports where people may be in danger, it is important to send officers.\n\nThis incident requires 2 officers for 2 turns, as indicated on the button below</t>
-  </si>
-  <si>
     <t>At the end of each turn, you are shown a summary of how well you have done.\n\nEvery turn has a number of incidents that you must review. Your 2 officers are still dispatched and won't return until another turn has been completed, as shown by the number on each officer icon.</t>
   </si>
   <si>
     <t>Tap here to start!</t>
+  </si>
+  <si>
+    <t>Ask citizens for help!</t>
+  </si>
+  <si>
+    <t>The top of the screen shows the current satisfaction status, the further into red you go, the closer you are to losing. Solve incidents to stay out of the red</t>
+  </si>
+  <si>
+    <t>This box will give you information on the current incident and keep you updated on its status</t>
+  </si>
+  <si>
+    <t>Each incident will need a number of officers to attend for a set number of turns</t>
+  </si>
+  <si>
+    <t>Each incident can have up to 3 options, wait for more officers, send the required officers or ask citizens for help when available</t>
+  </si>
+  <si>
+    <t>{0} Turn Survived\nEach turn will consist of a number of incidents with choices to make</t>
+  </si>
+  <si>
+    <t>{0} Turns Survived\nEach turn will consist of a number of incidents with choices to make</t>
+  </si>
+  <si>
+    <t>Checking For New Content…</t>
+  </si>
+  <si>
+    <t>In some incidents, you might not have enough information to act upon.\n\nTry asking citizens for some more information.</t>
+  </si>
+  <si>
+    <t>In Incidents where people may be in danger, it is important to send officers.\n\nThis incident requires 2 officers for 2 turns, as indicated on the button below</t>
+  </si>
+  <si>
+    <t>In Resource Force, It is your job to decide how to handle incoming incidents.\n\nMake sure to read each carefully, they may be best ignored.</t>
+  </si>
+  <si>
+    <t>Incident</t>
+  </si>
+  <si>
+    <t>Harassment</t>
+  </si>
+  <si>
+    <t>Incoming information of unidentified person harassing neighbours</t>
+  </si>
+  <si>
+    <t>Citizens provided a full descruption along with further information of assault, the exact location is unknown</t>
   </si>
 </sst>
 </file>
@@ -2041,8 +2041,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G110" sqref="G110"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2076,58 +2076,58 @@
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>471</v>
+      <c r="B2" s="11" t="s">
+        <v>464</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>120</v>
+      <c r="B3" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>533</v>
+      <c r="B4" s="11" t="s">
+        <v>518</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -2137,1582 +2137,1582 @@
         <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="11" t="s">
         <v>61</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="11" t="s">
         <v>49</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>482</v>
+      <c r="B11" s="11" t="s">
+        <v>519</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>91</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>451</v>
+      <c r="B25" s="11" t="s">
+        <v>445</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>130</v>
+      <c r="B27" s="11" t="s">
+        <v>126</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="11" t="s">
         <v>59</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>153</v>
+      <c r="B31" s="11" t="s">
+        <v>149</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>84</v>
+      <c r="B32" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>203</v>
+        <v>147</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>199</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>202</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>208</v>
+        <v>203</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>204</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>83</v>
+        <v>148</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>148</v>
+        <v>81</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>144</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="C43" s="7" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="C44" s="7" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>146</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>184</v>
+        <v>165</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>180</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>175</v>
+        <v>166</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>171</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>178</v>
+        <v>167</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>174</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B53" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="C53" s="7" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>179</v>
+        <v>169</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>175</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>177</v>
+        <v>170</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>173</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>177</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>202</v>
+        <v>179</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>198</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>183</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="11" t="s">
         <v>63</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>65</v>
+      <c r="B63" s="11" t="s">
+        <v>520</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="C64" s="7" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>72</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>521</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>522</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>200</v>
+        <v>69</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>196</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>450</v>
+        <v>141</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>444</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>443</v>
+        <v>142</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>437</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>442</v>
+        <v>143</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>436</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>523</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B75" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B75" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>438</v>
+        <v>107</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>432</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>432</v>
+        <v>108</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>426</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>143</v>
+        <v>111</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>139</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>162</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>137</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>138</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>411</v>
+        <v>150</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>405</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>410</v>
+        <v>151</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>404</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>408</v>
+        <v>154</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>402</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>409</v>
+        <v>152</v>
+      </c>
+      <c r="B88" s="11" t="s">
+        <v>403</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>407</v>
+        <v>153</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>401</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>405</v>
+        <v>155</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>524</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B91" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="C91" s="7" t="s">
         <v>406</v>
       </c>
-      <c r="C91" s="7" t="s">
-        <v>412</v>
-      </c>
       <c r="D91" s="5" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>163</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B93" s="5" t="s">
-        <v>192</v>
-      </c>
       <c r="C93" s="7" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B94" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>193</v>
+        <v>186</v>
+      </c>
+      <c r="B95" s="11" t="s">
+        <v>189</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>194</v>
+        <v>187</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>190</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
+      </c>
+      <c r="B97" s="11" t="s">
+        <v>195</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="4" t="s">
-        <v>467</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>468</v>
+        <v>460</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>461</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>0</v>
@@ -3723,13 +3723,13 @@
     </row>
     <row r="99" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="4" t="s">
-        <v>470</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>469</v>
+        <v>463</v>
+      </c>
+      <c r="B99" s="11" t="s">
+        <v>462</v>
       </c>
       <c r="C99" s="11" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>0</v>
@@ -3740,13 +3740,13 @@
     </row>
     <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
+      </c>
+      <c r="B100" s="11" t="s">
+        <v>206</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>0</v>
@@ -3757,13 +3757,13 @@
     </row>
     <row r="101" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>456</v>
+        <v>449</v>
+      </c>
+      <c r="B101" s="11" t="s">
+        <v>450</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>0</v>
@@ -3774,13 +3774,13 @@
     </row>
     <row r="102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>457</v>
+        <v>451</v>
+      </c>
+      <c r="B102" s="11" t="s">
+        <v>526</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>0</v>
@@ -3791,13 +3791,13 @@
     </row>
     <row r="103" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>460</v>
+        <v>452</v>
+      </c>
+      <c r="B103" s="11" t="s">
+        <v>453</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>0</v>
@@ -3808,13 +3808,13 @@
     </row>
     <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>462</v>
+        <v>454</v>
+      </c>
+      <c r="B104" s="11" t="s">
+        <v>455</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>0</v>
@@ -3825,13 +3825,13 @@
     </row>
     <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>464</v>
+        <v>456</v>
+      </c>
+      <c r="B105" s="11" t="s">
+        <v>457</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>0</v>
@@ -3842,418 +3842,418 @@
     </row>
     <row r="106" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>466</v>
+        <v>458</v>
+      </c>
+      <c r="B106" s="11" t="s">
+        <v>459</v>
       </c>
       <c r="C106" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>528</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A107" s="4" t="s">
+      <c r="B110" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="B111" s="11" t="s">
         <v>485</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="C111" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="B112" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A113" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="B113" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="B114" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A115" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="B115" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A116" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="B116" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="B117" s="11" t="s">
+        <v>493</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A118" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A108" s="4" t="s">
-        <v>486</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A109" s="4" t="s">
-        <v>487</v>
-      </c>
-      <c r="B109" s="5" t="s">
+      <c r="B118" s="11" t="s">
         <v>531</v>
       </c>
-      <c r="C109" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A110" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="B110" s="5" t="s">
+      <c r="C118" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A119" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="B119" s="11" t="s">
         <v>532</v>
       </c>
-      <c r="C110" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A111" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>495</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A112" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="B112" s="5" t="s">
+      <c r="C119" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A120" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="C112" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A113" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="B113" s="5" t="s">
+      <c r="B120" s="11" t="s">
         <v>497</v>
       </c>
-      <c r="C113" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A114" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="B114" s="5" t="s">
+      <c r="C120" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A121" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="C114" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A115" s="4" t="s">
+      <c r="B121" s="11" t="s">
+        <v>501</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A122" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="B115" s="5" t="s">
+      <c r="B122" s="11" t="s">
         <v>502</v>
       </c>
-      <c r="C115" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A116" s="4" t="s">
+      <c r="C122" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A123" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="B116" s="5" t="s">
+      <c r="B123" s="11" t="s">
         <v>503</v>
       </c>
-      <c r="C116" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A117" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="B117" s="5" t="s">
+      <c r="C123" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A124" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="C117" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A118" s="4" t="s">
+      <c r="B124" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A125" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="B118" s="5" t="s">
+      <c r="B125" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A126" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="B126" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A127" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="C118" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A119" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>509</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A120" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="B120" s="5" t="s">
+      <c r="B127" s="11" t="s">
+        <v>533</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A128" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="C120" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E120" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A121" s="4" t="s">
+      <c r="B128" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A129" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="B121" s="5" t="s">
+      <c r="B129" s="11" t="s">
         <v>514</v>
       </c>
-      <c r="C121" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A122" s="4" t="s">
+      <c r="C129" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A130" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="B130" s="11" t="s">
         <v>515</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A123" s="4" t="s">
-        <v>513</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A124" s="4" t="s">
-        <v>517</v>
-      </c>
-      <c r="B124" s="5" t="s">
-        <v>519</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A125" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>530</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A126" s="4" t="s">
-        <v>520</v>
-      </c>
-      <c r="B126" s="5" t="s">
-        <v>522</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E126" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A127" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="B127" s="5" t="s">
-        <v>523</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E127" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A128" s="4" t="s">
-        <v>524</v>
-      </c>
-      <c r="B128" s="5" t="s">
-        <v>527</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D128" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E128" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A129" s="4" t="s">
-        <v>525</v>
-      </c>
-      <c r="B129" s="5" t="s">
-        <v>528</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A130" s="4" t="s">
-        <v>526</v>
-      </c>
-      <c r="B130" s="5" t="s">
-        <v>529</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
update text to use a reference to game name rather than contain it in the text itself, helps to change in future
</commit_message>
<xml_diff>
--- a/Assets/Editor/Strings/StringFile.xlsx
+++ b/Assets/Editor/Strings/StringFile.xlsx
@@ -1559,9 +1559,6 @@
     <t>In Incidents where people may be in danger, it is important to send officers.\n\nThis incident requires 2 officers for 2 turns, as indicated on the button below</t>
   </si>
   <si>
-    <t>In Resource Force, It is your job to decide how to handle incoming incidents.\n\nMake sure to read each carefully, they may be best ignored.</t>
-  </si>
-  <si>
     <t>Incident</t>
   </si>
   <si>
@@ -1580,9 +1577,6 @@
     <t>0 Zaken genegeerd\n\nGeen verandering tevredenheid</t>
   </si>
   <si>
-    <t>In Resource Force is het jouw taak om te beslissen hoe inkomende rapporten verwerkt moeten worden. \n\nLees ieder rapport goed door, het kan ook genegeerd worden.</t>
-  </si>
-  <si>
     <t>In sommige gevallen heb je mogelijk niet genoeg informatie om op te treden. \n\nBetrek burgers om meer informatie te verzamelen.</t>
   </si>
   <si>
@@ -1712,9 +1706,6 @@
     <t>Introduce la dirección de correo electrónico para recibir las actualizaciones de INSPEC2T</t>
   </si>
   <si>
-    <t>Tu tarea en Resource Force es decidir cómo vas a gestionar los casos.\n\nAsegúrate de leer bien cada enunciado: algunos pueden ser ignorados.</t>
-  </si>
-  <si>
     <t>En algunos casos, puede que no tengas suficiente información para actuar.\n\nPregunta a la ciudadanía para obtener más detalles.</t>
   </si>
   <si>
@@ -1811,9 +1802,6 @@
     <t>Εισάγετε το email σας για να λαμβάνετε ενημερώσεις</t>
   </si>
   <si>
-    <t>Στο Resource Force, ο ρόλος σας είναι να διαχειριστείτε τις εισερχόμενες αναφορές.\n\nΔιαβάστε τις με προσοχή.</t>
-  </si>
-  <si>
     <t>Κάποιες αναφορές δεν έχουν επαρκεί στοιχεία.\n\nΖητήστε από τους πολίτες διευκρινήσεις</t>
   </si>
   <si>
@@ -1881,6 +1869,18 @@
   </si>
   <si>
     <t>Συγχαρητήρια. Πρέπει να αποσταλούν αστυνομικοί για να επιληφθούνε του συμβάντος</t>
+  </si>
+  <si>
+    <t>In {0}, It is your job to decide how to handle incoming incidents.\n\nMake sure to read each carefully, they may be best ignored.</t>
+  </si>
+  <si>
+    <t>In {0} is het jouw taak om te beslissen hoe inkomende rapporten verwerkt moeten worden. \n\nLees ieder rapport goed door, het kan ook genegeerd worden.</t>
+  </si>
+  <si>
+    <t>Στο {0}, ο ρόλος σας είναι να διαχειριστείτε τις εισερχόμενες αναφορές.\n\nΔιαβάστε τις με προσοχή.</t>
+  </si>
+  <si>
+    <t>Tu tarea en {0} es decidir cómo vas a gestionar los casos.\n\nAsegúrate de leer bien cada enunciado: algunos pueden ser ignorados.</t>
   </si>
 </sst>
 </file>
@@ -2264,8 +2264,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2303,13 +2303,13 @@
         <v>451</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2453,13 +2453,13 @@
         <v>36</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>461</v>
@@ -3448,7 +3448,7 @@
         <v>429</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
@@ -3465,7 +3465,7 @@
         <v>428</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3578,7 +3578,7 @@
         <v>421</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>419</v>
@@ -3595,13 +3595,13 @@
         <v>417</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>418</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3771,7 +3771,7 @@
         <v>408</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3788,7 +3788,7 @@
         <v>404</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3805,7 +3805,7 @@
         <v>403</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3822,7 +3822,7 @@
         <v>403</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3941,7 +3941,7 @@
         <v>278</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3955,10 +3955,10 @@
         <v>453</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3972,7 +3972,7 @@
         <v>454</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>205</v>
@@ -3989,10 +3989,10 @@
         <v>455</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4006,10 +4006,10 @@
         <v>456</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4023,10 +4023,10 @@
         <v>457</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4040,10 +4040,10 @@
         <v>458</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4057,10 +4057,10 @@
         <v>459</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4074,10 +4074,10 @@
         <v>460</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -4085,16 +4085,16 @@
         <v>462</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>511</v>
+        <v>615</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>518</v>
+        <v>616</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>595</v>
+        <v>617</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>562</v>
+        <v>618</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -4105,13 +4105,13 @@
         <v>509</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4122,13 +4122,13 @@
         <v>510</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4139,13 +4139,13 @@
         <v>500</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -4153,16 +4153,16 @@
         <v>466</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -4173,13 +4173,13 @@
         <v>470</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -4190,13 +4190,13 @@
         <v>471</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
@@ -4207,13 +4207,13 @@
         <v>472</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4221,13 +4221,13 @@
         <v>473</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>121</v>
@@ -4241,13 +4241,13 @@
         <v>476</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4258,13 +4258,13 @@
         <v>477</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4272,16 +4272,16 @@
         <v>478</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4289,16 +4289,16 @@
         <v>479</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4309,13 +4309,13 @@
         <v>481</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4326,13 +4326,13 @@
         <v>485</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4343,13 +4343,13 @@
         <v>486</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4360,13 +4360,13 @@
         <v>487</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4377,13 +4377,13 @@
         <v>490</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4394,13 +4394,13 @@
         <v>499</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4411,13 +4411,13 @@
         <v>493</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -4425,16 +4425,16 @@
         <v>492</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4442,16 +4442,16 @@
         <v>494</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4462,13 +4462,13 @@
         <v>497</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4479,13 +4479,13 @@
         <v>498</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run through branding process by creating lancs police version added functionality to enable/disable objects from the game Splash screen has to be set manually at the moment
</commit_message>
<xml_diff>
--- a/Assets/Editor/Strings/StringFile.xlsx
+++ b/Assets/Editor/Strings/StringFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="626">
   <si>
     <t>key</t>
   </si>
@@ -314,9 +314,6 @@
     <t>BASIC_TEXT_CHANGE_LOCATION</t>
   </si>
   <si>
-    <t>Change Location</t>
-  </si>
-  <si>
     <t>TUTORIAL_TEXT_HOW_TO_PLAY</t>
   </si>
   <si>
@@ -1881,13 +1878,37 @@
   </si>
   <si>
     <t>Tu tarea en {0} es decidir cómo vas a gestionar los casos.\n\nAsegúrate de leer bien cada enunciado: algunos pueden ser ignorados.</t>
+  </si>
+  <si>
+    <t>BRANDING_WELCOME_TEXT</t>
+  </si>
+  <si>
+    <t>BRANDING_DOWNLOAD_NOW</t>
+  </si>
+  <si>
+    <t>BRANDING_DOWNLOAD_MESSAGE</t>
+  </si>
+  <si>
+    <t>XXXX</t>
+  </si>
+  <si>
+    <t>Welcome to Resource Force - Lancashire, before you start, set your preferences for the best experience</t>
+  </si>
+  <si>
+    <t>Get In The Know Now!</t>
+  </si>
+  <si>
+    <t>Stay up to date with the things that concern you and your community!</t>
+  </si>
+  <si>
+    <t>Change Preferences</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1914,8 +1935,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1931,6 +1959,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1958,11 +1991,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1980,8 +2014,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2262,10 +2303,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2300,16 +2341,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2317,16 +2358,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2334,16 +2375,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2360,7 +2401,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2371,30 +2412,30 @@
         <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2405,13 +2446,13 @@
         <v>60</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2422,13 +2463,13 @@
         <v>49</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2439,13 +2480,13 @@
         <v>48</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2453,16 +2494,16 @@
         <v>36</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>543</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2473,13 +2514,13 @@
         <v>73</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2490,13 +2531,13 @@
         <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2507,13 +2548,13 @@
         <v>90</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2524,13 +2565,13 @@
         <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2541,13 +2582,13 @@
         <v>19</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2558,13 +2599,13 @@
         <v>20</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2575,13 +2616,13 @@
         <v>21</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2592,13 +2633,13 @@
         <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2609,13 +2650,13 @@
         <v>32</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2626,13 +2667,13 @@
         <v>25</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2643,13 +2684,13 @@
         <v>27</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2660,13 +2701,13 @@
         <v>29</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2680,10 +2721,10 @@
         <v>45</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -2691,16 +2732,16 @@
         <v>39</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="6" t="s">
         <v>434</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2711,13 +2752,13 @@
         <v>35</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2725,16 +2766,16 @@
         <v>34</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2745,13 +2786,13 @@
         <v>41</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2762,13 +2803,13 @@
         <v>47</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2779,13 +2820,13 @@
         <v>58</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2793,16 +2834,16 @@
         <v>43</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2813,81 +2854,81 @@
         <v>79</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>201</v>
-      </c>
       <c r="C34" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>203</v>
-      </c>
       <c r="C35" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2901,10 +2942,10 @@
         <v>55</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2918,10 +2959,10 @@
         <v>57</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2932,13 +2973,13 @@
         <v>51</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2949,13 +2990,13 @@
         <v>77</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2966,13 +3007,13 @@
         <v>52</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2980,16 +3021,16 @@
         <v>80</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3000,13 +3041,13 @@
         <v>85</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3017,13 +3058,13 @@
         <v>86</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3034,13 +3075,13 @@
         <v>84</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3051,13 +3092,13 @@
         <v>92</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3071,10 +3112,10 @@
         <v>94</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3082,186 +3123,186 @@
         <v>95</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>303</v>
+        <v>625</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="C49" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>176</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>182</v>
-      </c>
       <c r="C58" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3272,13 +3313,13 @@
         <v>75</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3289,30 +3330,30 @@
         <v>88</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="C61" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3323,13 +3364,13 @@
         <v>62</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3337,16 +3378,16 @@
         <v>63</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3357,13 +3398,13 @@
         <v>65</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3374,13 +3415,13 @@
         <v>71</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3388,16 +3429,16 @@
         <v>67</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3405,16 +3446,16 @@
         <v>70</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3422,67 +3463,67 @@
         <v>68</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="D70" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>428</v>
-      </c>
       <c r="E70" s="6" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3490,1002 +3531,1053 @@
         <v>69</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B74" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="C74" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="C76" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D77" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="E77" s="6" t="s">
         <v>419</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B78" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="D78" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>418</v>
-      </c>
       <c r="E78" s="6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B79" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B80" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="C80" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B81" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="C81" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B82" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="C82" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C86" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="E86" s="6" t="s">
         <v>412</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C88" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="D88" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="D88" s="4" t="s">
-        <v>408</v>
-      </c>
       <c r="E88" s="6" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C91" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D91" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="D91" s="4" t="s">
-        <v>403</v>
-      </c>
       <c r="E91" s="6" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B97" s="4" t="s">
-        <v>194</v>
-      </c>
       <c r="C97" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B98" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="B98" s="4" t="s">
-        <v>448</v>
-      </c>
       <c r="C98" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B100" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B100" s="4" t="s">
-        <v>205</v>
-      </c>
       <c r="C100" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B101" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="B101" s="4" t="s">
-        <v>437</v>
-      </c>
       <c r="C101" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B103" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="B103" s="4" t="s">
-        <v>440</v>
-      </c>
       <c r="C103" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="B104" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="B104" s="4" t="s">
-        <v>442</v>
-      </c>
       <c r="C104" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B105" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="B105" s="4" t="s">
-        <v>444</v>
-      </c>
       <c r="C105" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="B106" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="B106" s="4" t="s">
-        <v>446</v>
-      </c>
       <c r="C106" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B107" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="C107" s="4" t="s">
         <v>615</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="D107" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="E107" s="6" t="s">
         <v>617</v>
-      </c>
-      <c r="E107" s="6" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B111" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="C111" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="C111" s="4" t="s">
-        <v>521</v>
-      </c>
       <c r="D111" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A117" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A118" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A119" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B120" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="B120" s="4" t="s">
-        <v>481</v>
-      </c>
       <c r="C120" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A121" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A122" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A123" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A124" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A125" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A126" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A127" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B127" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="C127" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="C127" s="4" t="s">
-        <v>537</v>
-      </c>
       <c r="D127" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A128" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B128" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="C128" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="C128" s="4" t="s">
-        <v>539</v>
-      </c>
       <c r="D128" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A129" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A130" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>581</v>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A131" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A132" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A133" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lancashire assets and changes
</commit_message>
<xml_diff>
--- a/Assets/Editor/Strings/StringFile.xlsx
+++ b/Assets/Editor/Strings/StringFile.xlsx
@@ -1376,9 +1376,6 @@
     <t>BASIC_TEXT_SENT</t>
   </si>
   <si>
-    <t>Take on the role of a police operator and help to solve crimes across the city.\n\nKeep the city safe and citizens happy with the power of dispatch officers along with information from citizens.\n\nBut be careful, you only have a limited number of officers and citizens may not always provide good information</t>
-  </si>
-  <si>
     <t>Versturen</t>
   </si>
   <si>
@@ -1565,9 +1562,6 @@
     <t>Incoming information of unidentified person harassing neighbours</t>
   </si>
   <si>
-    <t>Stap in de rol van een politiechef en help misdaden in de stad op te lossen. Maak gebruik van de wijkagenten en de kracht van samenwerking met burgers om de stad veilig en burgers tevreden te houden! Wees voorzichtig, je hebt maar een beperkt aantal agenten en burgers dragen niet altijd op de juiste manier bij.</t>
-  </si>
-  <si>
     <t>{0} Zaak genegeerd {1}\n\n-{2}% Tevredenheid</t>
   </si>
   <si>
@@ -1655,9 +1649,6 @@
     <t>Vraag burgers om informatie!</t>
   </si>
   <si>
-    <t>Asume el papel de un agente de policía y resuelve los delitos en toda la ciudad.\n\nHaz un buen uso de la autoridad y también de la información de la ciudadanía para que estén felices y mantener la ciudad segura.\n\nPero ten cuidado: sólo tienes un número limitado de polícias y la población no siempre proporciona buena información.</t>
-  </si>
-  <si>
     <t>El botón de ignorar no enviará a ningún policía para que investigue el caso. \n\nUsa esto cuando no tengas disponibles suficientes policías o si el incidente exigiera demasiado. Pero utiliza esta opción con cuidado: los casos ignorados pueden empeorar mucho.</t>
   </si>
   <si>
@@ -1769,9 +1760,6 @@
     <t>¡Bien hecho! Es necesario enviar policías para asegurar de que nadie resulte herido</t>
   </si>
   <si>
-    <t>Αναλάβετε τον συντονιστικό ρόλο στην διάθεση αστυνομικών για την ασφάλεια της πόλης.\n\n Χρησιμοποιήστε τους διαθέσιμους αστυνόμους σε συνδυασμό με τις πληροφορίες από τους πολίτες.\n\n Προσοχή σας καθώς η δύναμη των διαθέσιμων αστυνομικών είναι περιορισμένη και οι πολίτες δεν αναφέρουν πάντα με ακρίβεια τα συμβάντα.</t>
-  </si>
-  <si>
     <t>Ρωτήστε τους πολίτες για πληροφορίες!</t>
   </si>
   <si>
@@ -1902,6 +1890,18 @@
   </si>
   <si>
     <t>Change Preferences</t>
+  </si>
+  <si>
+    <t>Take on the role of a police operator and help to solve crimes across the city.\n\nKeep the city safe and citizens happy with the power of dispatch officers along with information from citizens</t>
+  </si>
+  <si>
+    <t>Αναλάβετε τον συντονιστικό ρόλο στην διάθεση αστυνομικών για την ασφάλεια της πόλης.\n\n Χρησιμοποιήστε τους διαθέσιμους αστυνόμους σε συνδυασμό με τις πληροφορίες από τους πολίτες</t>
+  </si>
+  <si>
+    <t>Asume el papel de un agente de policía y resuelve los delitos en toda la ciudad.\n\nHaz un buen uso de la autoridad y también de la información de la ciudadanía para que estén felices y mantener la ciudad segura.</t>
+  </si>
+  <si>
+    <t>Stap in de rol van een politiechef en help misdaden in de stad op te lossen.\n\n Maak gebruik van de wijkagenten en de kracht van samenwerking met burgers om de stad veilig en burgers tevreden te houden!</t>
   </si>
 </sst>
 </file>
@@ -2305,8 +2305,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2336,21 +2336,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="102" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>450</v>
+        <v>622</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>513</v>
+        <v>625</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>581</v>
+        <v>623</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>543</v>
+        <v>624</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2375,7 +2375,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>327</v>
@@ -2494,16 +2494,16 @@
         <v>36</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3123,7 +3123,7 @@
         <v>95</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>363</v>
@@ -3378,7 +3378,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>378</v>
@@ -3429,7 +3429,7 @@
         <v>67</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>381</v>
@@ -3446,7 +3446,7 @@
         <v>70</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>382</v>
@@ -3489,7 +3489,7 @@
         <v>428</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
@@ -3506,7 +3506,7 @@
         <v>427</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3531,7 +3531,7 @@
         <v>69</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>384</v>
@@ -3619,7 +3619,7 @@
         <v>420</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>418</v>
@@ -3636,13 +3636,13 @@
         <v>416</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>417</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3812,7 +3812,7 @@
         <v>407</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3829,7 +3829,7 @@
         <v>403</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3837,7 +3837,7 @@
         <v>153</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>404</v>
@@ -3846,7 +3846,7 @@
         <v>402</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -3854,7 +3854,7 @@
         <v>154</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>401</v>
@@ -3863,7 +3863,7 @@
         <v>402</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3976,13 +3976,13 @@
         <v>447</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>277</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3993,13 +3993,13 @@
         <v>448</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4010,10 +4010,10 @@
         <v>204</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>204</v>
@@ -4027,13 +4027,13 @@
         <v>436</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4041,16 +4041,16 @@
         <v>437</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4061,13 +4061,13 @@
         <v>439</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4078,13 +4078,13 @@
         <v>441</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4095,13 +4095,13 @@
         <v>443</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4112,163 +4112,163 @@
         <v>445</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>120</v>
@@ -4276,308 +4276,308 @@
     </row>
     <row r="116" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A117" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A118" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A119" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="B120" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="B120" s="4" t="s">
-        <v>480</v>
-      </c>
       <c r="C120" s="4" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A121" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A122" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A123" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A124" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A125" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A126" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A127" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A128" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A129" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A130" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="B131" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="B131" s="3" t="s">
-        <v>622</v>
-      </c>
       <c r="C131" s="3" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="B132" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="B132" s="3" t="s">
-        <v>623</v>
-      </c>
       <c r="C132" s="3" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="B133" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="B133" s="3" t="s">
-        <v>624</v>
-      </c>
       <c r="C133" s="3" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>